<commit_message>
Advanced OCR v2.0: Image preprocessing + item extraction
</commit_message>
<xml_diff>
--- a/05-simple-ocr-client/output/delivery_notes.xlsx
+++ b/05-simple-ocr-client/output/delivery_notes.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Delivery Notes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Items Count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Review Status</t>
         </is>
       </c>
@@ -491,7 +496,10 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>
@@ -524,7 +532,10 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>
@@ -557,7 +568,10 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>

</xml_diff>

<commit_message>
Two ocr files created. simple and advanced.
</commit_message>
<xml_diff>
--- a/05-simple-ocr-client/output/delivery_notes.xlsx
+++ b/05-simple-ocr-client/output/delivery_notes.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Delivery Notes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,11 +461,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Items Count</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>Review Status</t>
         </is>
       </c>
@@ -496,10 +491,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>
@@ -532,10 +524,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>
@@ -568,10 +557,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>NEEDS REVIEW</t>
         </is>

</xml_diff>